<commit_message>
Fix Testing Strategy - Lab 9-10
</commit_message>
<xml_diff>
--- a/Лабораторная работа 9-10/Стратегия тестирования.xlsx
+++ b/Лабораторная работа 9-10/Стратегия тестирования.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-план" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="142">
   <si>
     <t>Тест-план по системному тестированию веб-приложения для доставки еды</t>
   </si>
@@ -76,27 +76,9 @@
     <t>Вывод списка блюд ресторана</t>
   </si>
   <si>
-    <t>На главной странице выводится список ресторанов из базы данных</t>
-  </si>
-  <si>
     <t>Авторизация клиента</t>
   </si>
   <si>
-    <t>Авторизация клиента проход успешно</t>
-  </si>
-  <si>
-    <t>Блюда добавляются из списка в корзину клиента, можно изменить количество товаров или очистить корзину</t>
-  </si>
-  <si>
-    <t>Авторизированному пользователю доступен список его совершенных заказов. По отправлению формы заказа, он появляется в этом списке.</t>
-  </si>
-  <si>
-    <t>Форма не отправляется без выполнения условий валидации. Данные заисываются в корректную таблицу БД.</t>
-  </si>
-  <si>
-    <t>На странице ресторана выводится список из соответсвующей БД.</t>
-  </si>
-  <si>
     <t>1 - Высший приоритет</t>
   </si>
   <si>
@@ -385,9 +367,6 @@
     <t>В поле "телефон" можно ввести только цифры и спец символы, нельзя ввести буквы</t>
   </si>
   <si>
-    <t>В списке всех ресторанов у каждого присутствует рейтинг, выведенный из БД</t>
-  </si>
-  <si>
     <t>В работе</t>
   </si>
   <si>
@@ -403,9 +382,6 @@
     <t>Minor</t>
   </si>
   <si>
-    <t>В поле ввода номера телефона не возможно ввести в распространенном формате</t>
-  </si>
-  <si>
     <t>Нет возможности ввести как +7 / должна быть</t>
   </si>
   <si>
@@ -427,24 +403,12 @@
     <t>Рейтинг визуально не выводится / должен выводиться</t>
   </si>
   <si>
-    <t>Статусы заказа могут быть непонятными / нечитаемыми для пользователей</t>
-  </si>
-  <si>
     <t>Статус на английском языке / должен быть на русском</t>
   </si>
   <si>
     <t>Протестирован, есть ошибки</t>
   </si>
   <si>
-    <t>Потестирован, есть ошибки</t>
-  </si>
-  <si>
-    <t>Протесирован, есть ошибки</t>
-  </si>
-  <si>
-    <t>Потестирован, нет ошибок</t>
-  </si>
-  <si>
     <t>Протестирован, нет ошибок</t>
   </si>
   <si>
@@ -463,34 +427,37 @@
     <t>Кошкин П.Н.</t>
   </si>
   <si>
-    <t>Проверка авторизации клиента в веб-приложении</t>
-  </si>
-  <si>
     <t>Дата</t>
   </si>
   <si>
-    <t>Проверка работы вывода списка ресторанов</t>
-  </si>
-  <si>
     <t>Описане теста:</t>
   </si>
   <si>
-    <t>Проверка функционала добавления, редактирования и удаления из корзины</t>
-  </si>
-  <si>
     <t>Луткова Д.В.</t>
   </si>
   <si>
-    <t>Список заказов пользователя совпадает с данными БД и показывает все данные о заказе</t>
-  </si>
-  <si>
-    <t>Форма заказа собирает все необходимые данные и отправляет в БД.</t>
-  </si>
-  <si>
-    <t>Проверка того, что все блюда из БД выводятся на странице ресторана</t>
-  </si>
-  <si>
     <t>Разработчик</t>
+  </si>
+  <si>
+    <t>Unit-тестирование модуля</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ручное тестирование модуля, проверка полноты выводимых данных </t>
+  </si>
+  <si>
+    <t>Ручное тестирование модуля, проверка валидации и работы с БД</t>
+  </si>
+  <si>
+    <t>Ручное тестирование модуля, проверка полноты выводимых данных</t>
+  </si>
+  <si>
+    <t>В списке всех ресторанов у каждого должен, но не присутствует рейтинг, выведенный из БД</t>
+  </si>
+  <si>
+    <t>Статусы заказа могут быть непонятными / нечитаемыми для пользователей из за отсутствия локализации</t>
+  </si>
+  <si>
+    <t>В поле ввода номера телефона не возможно ввести в распространенном формате (+7)</t>
   </si>
 </sst>
 </file>
@@ -971,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1036,10 +1003,10 @@
         <v>8</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1050,36 +1017,36 @@
         <v>1</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>148</v>
-      </c>
       <c r="H14" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="44" customHeight="1" x14ac:dyDescent="0.35">
@@ -1090,16 +1057,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="44" customHeight="1" x14ac:dyDescent="0.35">
@@ -1110,19 +1077,19 @@
         <v>2</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1130,16 +1097,16 @@
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="29" x14ac:dyDescent="0.35">
@@ -1150,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.35">
@@ -1168,7 +1135,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1152,169 @@
   <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="22">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,23 +1333,23 @@
     </row>
     <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C4" s="21">
         <v>2</v>
@@ -1228,283 +1357,121 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="22">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9">
         <v>43980</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
+    <row r="11" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="6" max="6" width="28.90625" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="25"/>
-    </row>
-    <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="2:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
@@ -1512,99 +1479,99 @@
     </row>
     <row r="15" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B16" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -1622,7 +1589,7 @@
   <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,43 +1602,43 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" s="25"/>
     </row>
     <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9">
         <v>43980</v>
@@ -1679,189 +1646,189 @@
     </row>
     <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="2:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1878,7 +1845,7 @@
   <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1891,29 +1858,29 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C1" s="25"/>
     </row>
     <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C4" s="21">
         <v>3</v>
@@ -1921,15 +1888,15 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="19" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C6" s="9">
         <v>43980</v>
@@ -1937,91 +1904,91 @@
     </row>
     <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="6" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
@@ -2040,280 +2007,6 @@
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="6" max="6" width="28.90625" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="25"/>
-    </row>
-    <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9">
-        <v>43980</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="2:7" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="2:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B16" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B19" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="2:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="B21" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2327,43 +2020,45 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C1" s="25"/>
     </row>
     <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="C4" s="21">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>148</v>
+        <v>128</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9">
         <v>43980</v>
@@ -2371,91 +2066,363 @@
     </row>
     <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B16" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="12" t="s">
         <v>80</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" spans="2:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="12" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -2472,7 +2439,7 @@
   <dimension ref="C1:G5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2486,36 +2453,36 @@
   <sheetData>
     <row r="1" spans="3:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C1" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="3:7" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="3:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2523,50 +2490,50 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="5">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2592,21 +2559,21 @@
   <sheetData>
     <row r="1" spans="4:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D1" s="26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E1" s="26"/>
     </row>
     <row r="2" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E3" s="14">
         <v>43980</v>
@@ -2614,15 +2581,15 @@
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D6" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E6" s="5">
         <v>53</v>
@@ -2631,7 +2598,7 @@
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E7" s="5">
         <v>53</v>
@@ -2642,24 +2609,24 @@
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D8" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E8" s="5">
         <v>49</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E9" s="5">
         <v>4</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.35">
@@ -2667,7 +2634,7 @@
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D11" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E11" s="5">
         <v>4</v>
@@ -2675,7 +2642,7 @@
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D12" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -2683,7 +2650,7 @@
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D13" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -2691,7 +2658,7 @@
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -2699,7 +2666,7 @@
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D15" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -2707,7 +2674,7 @@
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D16" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2715,12 +2682,12 @@
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D19" s="27" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>

</xml_diff>